<commit_message>
sdfsdf gfdsgsd sdfgfsdg sdfsdf
</commit_message>
<xml_diff>
--- a/word/word.xlsx
+++ b/word/word.xlsx
@@ -123,10 +123,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -144,23 +144,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -173,9 +187,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,24 +202,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,6 +241,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -252,8 +265,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -261,21 +275,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -290,187 +290,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,17 +499,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,26 +523,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -588,11 +567,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -604,10 +604,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -616,137 +616,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -758,9 +758,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1117,7 +1114,7 @@
   <sheetPr/>
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1137,10 +1134,10 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1148,10 +1145,10 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1159,10 +1156,10 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1170,10 +1167,10 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1181,10 +1178,10 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1192,10 +1189,10 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1203,10 +1200,10 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1214,10 +1211,10 @@
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1225,10 +1222,10 @@
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1236,10 +1233,10 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1247,10 +1244,10 @@
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1258,10 +1255,10 @@
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1269,288 +1266,288 @@
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" customHeight="1" spans="1:3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" customHeight="1" spans="1:3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="2"/>
     </row>
     <row r="17" customHeight="1" spans="1:3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" customHeight="1" spans="1:3">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" customHeight="1" spans="1:3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" customHeight="1" spans="1:3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" customHeight="1" spans="1:3">
       <c r="A21" s="2">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="2"/>
     </row>
     <row r="22" customHeight="1" spans="1:3">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="2"/>
     </row>
     <row r="23" customHeight="1" spans="1:3">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
     </row>
     <row r="24" customHeight="1" spans="1:3">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
     </row>
     <row r="25" customHeight="1" spans="1:3">
       <c r="A25" s="2">
         <v>24</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
     </row>
     <row r="26" customHeight="1" spans="1:3">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" customHeight="1" spans="1:3">
       <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
     </row>
     <row r="28" customHeight="1" spans="1:3">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" customHeight="1" spans="1:3">
       <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
     </row>
     <row r="30" customHeight="1" spans="1:3">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
     </row>
     <row r="31" customHeight="1" spans="1:3">
       <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
     </row>
     <row r="32" customHeight="1" spans="1:3">
       <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" customHeight="1" spans="1:3">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" customHeight="1" spans="1:3">
       <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" customHeight="1" spans="1:3">
       <c r="A35" s="2">
         <v>34</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
     </row>
     <row r="36" customHeight="1" spans="1:3">
       <c r="A36" s="2">
         <v>35</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
     </row>
     <row r="37" customHeight="1" spans="1:3">
       <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
     </row>
     <row r="38" customHeight="1" spans="1:3">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
     </row>
     <row r="39" customHeight="1" spans="1:3">
       <c r="A39" s="2">
         <v>38</v>
       </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
     </row>
     <row r="40" customHeight="1" spans="1:3">
       <c r="A40" s="2">
         <v>39</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" customHeight="1" spans="1:3">
       <c r="A41" s="2">
         <v>40</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
     </row>
     <row r="42" customHeight="1" spans="1:3">
       <c r="A42" s="2">
         <v>41</v>
       </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
     </row>
     <row r="43" customHeight="1" spans="1:3">
       <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" customHeight="1" spans="1:3">
       <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
     </row>
     <row r="45" customHeight="1" spans="1:3">
       <c r="A45" s="2">
         <v>44</v>
       </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
     </row>
     <row r="46" customHeight="1" spans="1:3">
       <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
     </row>
     <row r="47" customHeight="1" spans="1:3">
       <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
     </row>
     <row r="48" customHeight="1" spans="1:3">
       <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
     </row>
     <row r="49" customHeight="1" spans="1:3">
       <c r="A49" s="2">
         <v>48</v>
       </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
     </row>
     <row r="50" customHeight="1" spans="1:3">
       <c r="A50" s="2">
         <v>49</v>
       </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
     </row>
     <row r="51" customHeight="1" spans="1:3">
       <c r="A51" s="2">
         <v>50</v>
       </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B51 B52:B1048576">
+  <conditionalFormatting sqref="B:B">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>AND(COUNTIF($B:$B,B1)&gt;1,NOT(ISBLANK(B1)))</formula>
     </cfRule>

</xml_diff>